<commit_message>
Fitness y and index completos, pruebas listas
</commit_message>
<xml_diff>
--- a/Datos/Bomberos.xlsx
+++ b/Datos/Bomberos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielHernandezCuero\Documents\GeneticAlgorithm\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A1471BE9-F76F-4D0D-BC02-ED923AD472D8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{17192D44-9FAA-47B0-9115-25E6CFDF793D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{E9CAEBD5-B904-4E59-A479-356BC038FACD}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +85,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color rgb="FF4285F4"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -107,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -118,6 +125,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{009D6DF0-8D24-4E5A-9B95-E3DEBE8EE1FD}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +452,7 @@
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -454,7 +463,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -465,7 +474,7 @@
         <v>3.4921310000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -476,7 +485,7 @@
         <v>3.4908410000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -487,7 +496,7 @@
         <v>3.4638239999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -498,7 +507,7 @@
         <v>3.46061</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -509,7 +518,7 @@
         <v>3.4483290000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -520,7 +529,7 @@
         <v>3.436747</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -531,18 +540,19 @@
         <v>3.4275380000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>-76.517653999999993</v>
+        <v>-76.517751000000004</v>
       </c>
       <c r="C9" s="1">
-        <v>3.4118400000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.4107189999999998</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -553,7 +563,7 @@
         <v>3.4175800000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -563,6 +573,9 @@
       <c r="C11" s="1">
         <v>3.4596610000000001</v>
       </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>